<commit_message>
Update Glosario violencia de género .xlsx
</commit_message>
<xml_diff>
--- a/Glosario violencia de género .xlsx
+++ b/Glosario violencia de género .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Arancibia\Dropbox\Diseño DATA's (1)\DATA-RIESGOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{BD475410-E771-F943-996E-BD02DA04E81A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C00B61CC-EC6E-4084-B8FE-DB46336FF2F6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0C9B4D-E3FA-441B-94E6-0DB7F04BE288}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E1ED9E99-B3DD-E94F-A49F-A85F76739F82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E1ED9E99-B3DD-E94F-A49F-A85F76739F82}"/>
   </bookViews>
   <sheets>
     <sheet name="GLOSARIO VIOLENCIA DE GÉNERO" sheetId="1" r:id="rId1"/>
@@ -63,24 +63,9 @@
     <t xml:space="preserve">Violencia intrafamiliar </t>
   </si>
   <si>
-    <t>La violencia intrafamiliar (VIF) en Chile, corresponde a todo maltrato que afecte a la
-vida o la integridad física o psíquica de la víctima.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La violencia sexual se manifiesta de diversas formas: física, simbólica, explícita o
-implícitamente, y corresponde a cualquier práctica que atente contra el desarrollo pleno
-de la sexualidad de las mujeres. Como expresión del continuo de violencia, está presente
-desde la infancia y se manifiesta en diversos espacios: familia, instituciones educativas,
-religiosas, laborales, espacios públicos, centros de salud, etc. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Violencia Institucional </t>
   </si>
   <si>
-    <t xml:space="preserve">La violencia institucional corresponde a las manifestaciones de violencia patriarcal al interior de instituciones, tanto públicas como privadas. El Estado y sus aparatos es uno de los principales productores y reproductores de este tipo de violencia. El Poder Judicial, legislativo y ejecutivo son sostenedores de políticas públicas deficientes, del no reconocimiento de los derechos humanos de las mujeres y de un actuar negligente
-cuando se trata de garantizar vidas libres de violencia para mujeres y niñas. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Femicidio - Parricidio </t>
   </si>
   <si>
@@ -114,9 +99,6 @@
     <t xml:space="preserve">Suicidio femicida </t>
   </si>
   <si>
-    <t xml:space="preserve">Se trata de mujeres que son impulsadas al suicidio como consecuencia del acoso y la violencia constante a la que se ven sometidas considerando el suicido como "única salida . También como medida desesperada para poner fin a los malos tratos o como señal de impotencia frente a la impunidad en que se desenvuelve su agresor. </t>
-  </si>
-  <si>
     <t>Se entenderá por femicidio el asesinato de mujeres por razones asociadas con su género. El femicidio es la forma más extrema de violencia de género, entendida esta como la violencia ejercida por los hombres contra las mujeres en su deseo de obtener poder, dominación o control. Incluye los asesinatos producidos por la violencia intrafamiliar y la violencia sexual. El femicidio puede tomar dos formas: femicidio íntimo o femicidio no íntimo.</t>
   </si>
   <si>
@@ -127,6 +109,19 @@
   </si>
   <si>
     <t>Descripción</t>
+  </si>
+  <si>
+    <t>La violencia institucional corresponde a las manifestaciones de violencia patriarcal al interior de instituciones, tanto públicas como privadas. El Estado y sus aparatos es uno de los principales productores y reproductores de este tipo de violencia. El Poder Judicial, legislativo y ejecutivo son sostenedores de políticas públicas deficientes, del no reconocimiento de los derechos humanos de las mujeres y de un actuar negligente cuando se trata de garantizar vidas libres de violencia para mujeres y niñas.</t>
+  </si>
+  <si>
+    <t>La violencia sexual se manifiesta de diversas formas: física, simbólica, explícita o implícitamente, y corresponde a cualquier práctica que atente contra el desarrollo pleno
+de la sexualidad de las mujeres. Como expresión del continuo de violencia, está presente desde la infancia y se manifiesta en diversos espacios: familia, instituciones educativas, religiosas, laborales, espacios públicos, centros de salud, etc.</t>
+  </si>
+  <si>
+    <t>La violencia intrafamiliar (VIF) en Chile, corresponde a todo maltrato que afecte a la vida o la integridad física o psíquica de la víctima.</t>
+  </si>
+  <si>
+    <t>Se trata de mujeres que son impulsadas al suicidio como consecuencia del acoso y la violencia constante a la que se ven sometidas considerando el suicido como "única salida". También como medida desesperada para poner fin a los malos tratos o como señal de impotencia frente a la impunidad en que se desenvuelve su agresor.</t>
   </si>
 </sst>
 </file>
@@ -183,7 +178,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -194,6 +196,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9959D5BD-75D9-4ED6-92C5-4F02D78BE2E9}" name="Glosario_Femicidios_CL" displayName="Glosario_Femicidios_CL" ref="A1:B16" totalsRowShown="0">
+  <autoFilter ref="A1:B16" xr:uid="{AE8D6DF7-E9FC-4417-B0AE-580C49304DAE}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A9CBEF99-0A90-466E-A5F4-191260AFA6E7}" name="Concepto" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{F589B200-EE33-4B64-99C0-1608171B0F87}" name="Descripción" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -495,31 +508,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B99A33-A391-DB4A-A4F4-728A49AB752A}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.796875" customWidth="1"/>
+    <col min="1" max="1" width="25.75" customWidth="1"/>
     <col min="2" max="2" width="126.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="82.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="82.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -527,7 +542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -535,7 +550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -543,23 +558,23 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="78" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="63" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -567,71 +582,74 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="63" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="4" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="16" spans="1:2" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>